<commit_message>
Arreglat FiveDigits i Excels
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/100101/Resultats.xlsx
+++ b/TFG/res/pacientData/100101/Resultats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="523">
   <si>
     <t>ID</t>
   </si>
@@ -1544,10 +1544,43 @@
     <t>Home</t>
   </si>
   <si>
+    <t>Només castellà</t>
+  </si>
+  <si>
+    <t>22/06/2017</t>
+  </si>
+  <si>
     <t>Universitari grau mig</t>
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>Casat</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>Científic/intel·lectual</t>
+  </si>
+  <si>
+    <t>Pensionista</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>Ara no, anteriorment sí (fa més de 12 mesos que no en fa)</t>
   </si>
 </sst>
 </file>
@@ -3414,16 +3447,64 @@
         <v>509</v>
       </c>
       <c r="D2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F2" t="s">
+        <v>512</v>
+      </c>
+      <c r="G2" t="s">
+        <v>513</v>
+      </c>
+      <c r="H2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I2" t="s">
+        <v>515</v>
+      </c>
+      <c r="J2" t="s">
+        <v>516</v>
+      </c>
+      <c r="K2" t="s">
+        <v>517</v>
+      </c>
+      <c r="L2" t="s">
+        <v>518</v>
+      </c>
+      <c r="M2" t="s">
+        <v>519</v>
+      </c>
+      <c r="N2" t="s">
+        <v>520</v>
+      </c>
+      <c r="O2" t="s">
+        <v>520</v>
+      </c>
+      <c r="P2" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q2" t="s">
         <v>137</v>
       </c>
-      <c r="E2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" t="s">
-        <v>510</v>
-      </c>
-      <c r="G2" t="s">
-        <v>511</v>
+      <c r="R2" t="s">
+        <v>520</v>
+      </c>
+      <c r="S2" t="s">
+        <v>521</v>
+      </c>
+      <c r="T2" t="s">
+        <v>520</v>
+      </c>
+      <c r="U2" t="s">
+        <v>520</v>
+      </c>
+      <c r="V2" t="s">
+        <v>520</v>
+      </c>
+      <c r="W2" t="s">
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>